<commit_message>
Ned fix(products): create multi table
</commit_message>
<xml_diff>
--- a/new_Teste_pandas.xlsx
+++ b/new_Teste_pandas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,114 +436,338 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Dia</t>
+          <t>DIA</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>TA</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>F9TA</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>F9PLTA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>F12TA</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>F14TA</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>F18TA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>F18PLTA</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>F24PLTA</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>F1869TA</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>F9TB</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>F9PLTB</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>F12TB</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>F14TB</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>F18TB</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>F18PLTB</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>F24PLTB</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>F1869TB</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>TC</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>F9TC</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>F9PLTC</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>F12TC</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>F14TC</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>F18TC</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>F18PLTC</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>F24PLTC</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>F1869TC</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
           <t>F9</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>f12</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>f14</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>F9PL</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>F12</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>F1269</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>F14</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>F24</t>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>F18</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>F18PL</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>F24PL</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>F1869</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
-        <v>30</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
-        <v>25</v>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>110</v>
+      </c>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>35</v>
-      </c>
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>10</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>[{}]</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="n">
         <v>15</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>2</v>
-      </c>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>